<commit_message>
Iteración 1 de la entrega 5 terminada.
</commit_message>
<xml_diff>
--- a/Recursos/Puntuaciones.xlsx
+++ b/Recursos/Puntuaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo Fin Grado\Repositorio\TFG\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D178760-B4F6-40A9-93AA-D11067638D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B355EF-039D-4D82-8440-CDADF60FDA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31910" yWindow="-340" windowWidth="28800" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33250" yWindow="480" windowWidth="28800" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -86,19 +86,19 @@
     <t>Helena</t>
   </si>
   <si>
-    <t>Antonio</t>
-  </si>
-  <si>
-    <t>Papá</t>
-  </si>
-  <si>
-    <t>Mamá</t>
-  </si>
-  <si>
-    <t>Hermana</t>
-  </si>
-  <si>
-    <t>Madre Helena</t>
+    <t>Madre Helena (A)</t>
+  </si>
+  <si>
+    <t>Papá (B)</t>
+  </si>
+  <si>
+    <t>Mamá (C)</t>
+  </si>
+  <si>
+    <t>Hermana (D)</t>
+  </si>
+  <si>
+    <t>Antonio (E)</t>
   </si>
 </sst>
 </file>
@@ -447,12 +447,12 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" customWidth="1"/>
@@ -539,98 +539,243 @@
         <v>50</v>
       </c>
       <c r="Q2" s="5">
-        <f>SUM(O2:O7)/6</f>
-        <v>50</v>
+        <f>SUM(O3:O7)/5</f>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
       <c r="M3" s="4">
         <f t="shared" ref="M3:M7" si="0">(B3+D3+F3+H3+J3)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" ref="N3:N7" si="1">C3+E3+G3+I3+K3</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" ref="O3:O7" si="2">((M3-5)+(25-N3))*2.5</f>
-        <v>50</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
       <c r="M4" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="N4" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O4" s="4">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
       <c r="M5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="N5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O5" s="4">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
       <c r="M6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="N6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O6" s="4">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
       <c r="M7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O7" s="4">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cuestionarios y pruebas de la iteración 2 de la entrega 5
</commit_message>
<xml_diff>
--- a/Recursos/Puntuaciones.xlsx
+++ b/Recursos/Puntuaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trabajo Fin Grado\Repositorio\TFG\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B355EF-039D-4D82-8440-CDADF60FDA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E244D9DD-33D5-44F4-AF98-0ACBE475E1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33250" yWindow="480" windowWidth="28800" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19470" yWindow="11235" windowWidth="15345" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Media SUS</t>
   </si>
   <si>
-    <t>Helena</t>
-  </si>
-  <si>
     <t>Madre Helena (A)</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Antonio (E)</t>
+  </si>
+  <si>
+    <t>Helena (F)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -545,7 +545,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4">
         <v>5</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>

</xml_diff>